<commit_message>
Added nav bar for sep forms, fixed label printing to two sheets. Heavy refactoring
</commit_message>
<xml_diff>
--- a/assets/LabelTemplate.xlsx
+++ b/assets/LabelTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abu89\PycharmProjects\SAPAutomation\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9860EAF7-E038-4C79-BE22-FA993AE19635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58441FBE-7FED-476A-995F-29B208AB0D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED06BA1C-D3EC-48C4-8FBF-B9849328BAB1}"/>
+    <workbookView xWindow="1665" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{ED06BA1C-D3EC-48C4-8FBF-B9849328BAB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,8 +71,13 @@
     </font>
     <font>
       <sz val="36"/>
+      <name val="Arial Nova Cond"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="36"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial Nova Cond"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -78,12 +90,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -91,20 +103,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,85 +454,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630BCF46-A068-48F4-AF98-30974067DBC0}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="45.75" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:1" ht="45.75" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="3" spans="1:1" ht="45.75" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.6">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="A3:E4"/>
-    <mergeCell ref="A5:E6"/>
-    <mergeCell ref="A7:E8"/>
-  </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="259" fitToWidth="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>